<commit_message>
CENG407 SRS file completed
</commit_message>
<xml_diff>
--- a/Documents/WorkPlan/Work_Planceng407.xlsx
+++ b/Documents/WorkPlan/Work_Planceng407.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Masaüstü\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ceng407\ceng-407-408-2024-2025-EmoTagger-A-Community-driven-Emotion-Annotation-Tool\Documents\WorkPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33465D37-5022-41FD-A0EA-1D96AE94247A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89416F92-5505-4BAF-8049-5956213EEFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
-    <t>Start Date 24/10/2023</t>
-  </si>
-  <si>
     <t xml:space="preserve">Week                                                              </t>
   </si>
   <si>
@@ -116,13 +113,16 @@
   </si>
   <si>
     <t>13 January 2024</t>
+  </si>
+  <si>
+    <t>Start Date 30/09/2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -173,30 +173,48 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6AA84F"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="7"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="7"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="7"/>
       <name val="Söhne"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF6AA84F"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="18">
@@ -315,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -332,7 +350,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -340,16 +357,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -360,6 +374,12 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,8 +600,8 @@
   </sheetPr>
   <dimension ref="B2:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -591,14 +611,14 @@
     <col min="3" max="3" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20">
+    <row r="2" spans="2:20" ht="13.2">
       <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" ht="13.2" outlineLevel="1">
+      <c r="B3" s="2" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:20" outlineLevel="1">
-      <c r="B3" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3">
@@ -651,179 +671,179 @@
       </c>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="2:20">
+    <row r="4" spans="2:20" ht="13.2">
       <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" ht="13.2">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="2:20">
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="2:20" ht="13.2">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="2:20">
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="2:20" ht="13.2">
+      <c r="B7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="2:20">
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="2:20" ht="13.2">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="2:20">
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="2:20" ht="13.2">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="20"/>
+    </row>
+    <row r="10" spans="2:20" ht="13.2">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="2:20">
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="22"/>
-    </row>
-    <row r="10" spans="2:20">
-      <c r="B10" s="1" t="s">
+      <c r="I10" s="15"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+    </row>
+    <row r="11" spans="2:20" ht="13.2">
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-    </row>
-    <row r="11" spans="2:20">
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+    </row>
+    <row r="12" spans="2:20" ht="13.2">
+      <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-    </row>
-    <row r="12" spans="2:20">
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="21"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+    </row>
+    <row r="13" spans="2:20" ht="13.2">
+      <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M12" s="23"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-    </row>
-    <row r="13" spans="2:20">
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="24"/>
+    </row>
+    <row r="14" spans="2:20" ht="13.2">
+      <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="26"/>
-    </row>
-    <row r="14" spans="2:20">
-      <c r="B14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
-      <c r="S14" s="28"/>
+      <c r="C14" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="S14" s="26"/>
     </row>
     <row r="15" spans="2:20" ht="15.75" customHeight="1">
-      <c r="R15" s="29"/>
-      <c r="S15" s="29"/>
+      <c r="R15" s="27"/>
+      <c r="S15" s="27"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>